<commit_message>
Add MTOW restrictions for brake energy, Flaps TO/APPR and no anti-ice
Added the MTOW restriction calculated fields for brake energy, Flaps TO/APPR, no anti-ice.

Added some minor data validation.

Added Flaps & Anti-Ice input fields, nothing in the backend yet.
</commit_message>
<xml_diff>
--- a/HondaJet Perf Calc.xlsx
+++ b/HondaJet Perf Calc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Documents\HondaJet Perf Calc\hjet-performance-calculator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{409BBCC4-D947-405C-9B64-32FDD419F1AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E00D47-2A1F-4CA1-8B7B-E0F1BB8F7B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{63ACE541-7DEF-4A6E-868E-15DE9EBE8715}"/>
   </bookViews>
@@ -20,6 +20,16 @@
     <sheet name="AdminTools" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="TO_MTOWBrake_TO_NoAI_1000">'MTOW Brake Energy'!$A$3:$B$7</definedName>
+    <definedName name="TO_MTOWBrake_TO_NoAI_10000">'MTOW Brake Energy'!$A$253:$B$313</definedName>
+    <definedName name="TO_MTOWBrake_TO_NoAI_2000">'MTOW Brake Energy'!$A$11:$B$19</definedName>
+    <definedName name="TO_MTOWBrake_TO_NoAI_3000">'MTOW Brake Energy'!$A$23:$B$35</definedName>
+    <definedName name="TO_MTOWBrake_TO_NoAI_4000">'MTOW Brake Energy'!$A$39:$B$56</definedName>
+    <definedName name="TO_MTOWBrake_TO_NoAI_5000">'MTOW Brake Energy'!$A$60:$B$82</definedName>
+    <definedName name="TO_MTOWBrake_TO_NoAI_6000">'MTOW Brake Energy'!$A$86:$B$112</definedName>
+    <definedName name="TO_MTOWBrake_TO_NoAI_7000">'MTOW Brake Energy'!$A$116:$B$147</definedName>
+    <definedName name="TO_MTOWBrake_TO_NoAI_8000">'MTOW Brake Energy'!$A$151:$B$193</definedName>
+    <definedName name="TO_MTOWBrake_TO_NoAI_9000">'MTOW Brake Energy'!$A$197:$B$249</definedName>
     <definedName name="TO_MTOWClimb_TO_NoAI_0">'MTOW Climb Requirements'!$A$16:$B$25</definedName>
     <definedName name="TO_MTOWClimb_TO_NoAI_1000">'MTOW Climb Requirements'!$A$29:$B$39</definedName>
     <definedName name="TO_MTOWClimb_TO_NoAI_10000">'MTOW Climb Requirements'!$A$198:$B$217</definedName>
@@ -94,7 +104,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1042" uniqueCount="126">
   <si>
     <t>Uncorrected Takeoff Field Length [ft] and Speeds [KIAS], Dry Runway, Zero Slope, No Wind</t>
   </si>
@@ -436,9 +446,6 @@
     <t>MTOW Limitation (Climb)</t>
   </si>
   <si>
-    <t>Calculated Bracket MTOWs (Climb)</t>
-  </si>
-  <si>
     <t>TW / CW Bracket [TOFL]</t>
   </si>
   <si>
@@ -449,6 +456,33 @@
   </si>
   <si>
     <t>MTOW for Climb Requirements (Temperatures, MTOW)</t>
+  </si>
+  <si>
+    <t>Calculated Bracket MTOWs (Climb &amp; Brake)</t>
+  </si>
+  <si>
+    <t>MTOW Limitation (Brake)</t>
+  </si>
+  <si>
+    <t>Flaps</t>
+  </si>
+  <si>
+    <t>Anti-Ice</t>
+  </si>
+  <si>
+    <t>Data Validation Lists</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>OFF</t>
+  </si>
+  <si>
+    <t>TO/APPR</t>
+  </si>
+  <si>
+    <t>UP</t>
   </si>
 </sst>
 </file>
@@ -576,7 +610,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -651,11 +685,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -730,10 +773,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -742,28 +799,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -778,8 +820,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1185,7 +1233,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1194,12 +1242,14 @@
     <col min="2" max="2" width="10.42578125" customWidth="1"/>
     <col min="4" max="4" width="31" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" customWidth="1"/>
-    <col min="6" max="6" width="30.85546875" customWidth="1"/>
-    <col min="7" max="7" width="22.5703125" customWidth="1"/>
+    <col min="6" max="6" width="32.42578125" customWidth="1"/>
+    <col min="7" max="7" width="31.42578125" customWidth="1"/>
     <col min="8" max="8" width="10.85546875" customWidth="1"/>
     <col min="9" max="9" width="31" customWidth="1"/>
-    <col min="10" max="10" width="8.5703125" customWidth="1"/>
-    <col min="11" max="15" width="13.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="12" max="12" width="23.140625" customWidth="1"/>
+    <col min="13" max="15" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1207,7 +1257,7 @@
         <v>4</v>
       </c>
       <c r="B1" s="21">
-        <v>9000</v>
+        <v>10600</v>
       </c>
       <c r="D1" s="20" t="s">
         <v>40</v>
@@ -1221,28 +1271,46 @@
 B1&lt;= 10300, 10000,
 B1 &lt;= 10600, 10600,
 B1 &gt; 10600, "ABOVE MTOW")</f>
-        <v>9000</v>
-      </c>
-      <c r="H1" s="40" t="s">
-        <v>113</v>
-      </c>
-      <c r="I1" s="40"/>
+        <v>10600</v>
+      </c>
+      <c r="H1" s="57" t="s">
+        <v>117</v>
+      </c>
+      <c r="I1" s="58"/>
+      <c r="J1" s="58"/>
+      <c r="L1" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
+      <c r="A2" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="B2" s="21"/>
       <c r="D2" s="20"/>
       <c r="E2" s="37"/>
       <c r="H2" s="3">
         <f>$E$4</f>
         <v>6000</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="32">
         <f ca="1">IFERROR(
 IF(
 B10&lt;= INDEX(INDIRECT(F4), 1, 2),
 INDEX(INDIRECT(F4), 2, 2),
 VLOOKUP(B10,INDIRECT(F4),2,FALSE)), "Not within documented limits")</f>
-        <v>8350</v>
+        <v>7500</v>
+      </c>
+      <c r="J2" s="32">
+        <f ca="1">IFERROR(
+IF(
+B10&lt;= INDEX(INDIRECT(G4), 1, 2),
+INDEX(INDIRECT(G4), 2, 2),
+VLOOKUP(B10,INDIRECT(G4),2,FALSE)), "Not within documented limits")</f>
+        <v>9246.6666666666679</v>
+      </c>
+      <c r="L2" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1274,17 +1342,40 @@
 E3=10000, "TO_MTOWClimb_TO_NoAI_10000"), "No Table Available")</f>
         <v>TO_MTOWClimb_TO_NoAI_6000</v>
       </c>
-      <c r="G3" s="20"/>
+      <c r="G3" s="59" t="str" cm="1">
+        <f t="array" ref="G3">IFERROR(_xlfn.IFS(E3 = 1000, "TO_MTOWBrake_TO_NoAI_1000",
+E3 = 2000, "TO_MTOWBrake_TO_NoAI_2000",
+E3= 3000, "TO_MTOWBrake_TO_NoAI_3000",
+E3=4000, "TO_MTOWBrake_TO_NoAI_4000",
+E3=5000, "TO_MTOWBrake_TO_NoAI_5000",
+E3=6000, "TO_MTOWBrake_TO_NoAI_6000",
+E3=7000, "TO_MTOWBrake_TO_NoAI_7000",
+E3=8000, "TO_MTOWBrake_TO_NoAI_8000",
+E3=9000, "TO_MTOWBrake_TO_NoAI_9000",
+E3=10000, "TO_MTOWBrake_TO_NoAI_10000"), "No Table Available")</f>
+        <v>TO_MTOWBrake_TO_NoAI_6000</v>
+      </c>
       <c r="H3" s="3">
         <f>($E$4-(125*1))</f>
         <v>5875</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="32">
         <f ca="1">((I2-I4) / 2) + I4</f>
-        <v>8437.5</v>
+        <v>7593.75</v>
+      </c>
+      <c r="J3" s="32">
+        <f ca="1">((J2-J4) / 2) + J4</f>
+        <v>9291.6666666666679</v>
+      </c>
+      <c r="L3" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" s="21"/>
       <c r="D4" s="20" t="s">
         <v>106</v>
       </c>
@@ -1307,14 +1398,30 @@
 E4=10000, "TO_MTOWClimb_TO_NoAI_10000"), "No Table Available")</f>
         <v>TO_MTOWClimb_TO_NoAI_6000</v>
       </c>
-      <c r="G4" s="20"/>
+      <c r="G4" s="59" t="str" cm="1">
+        <f t="array" ref="G4">IFERROR(_xlfn.IFS(E4 = 1000, "TO_MTOWBrake_TO_NoAI_1000",
+E4 = 2000, "TO_MTOWBrake_TO_NoAI_2000",
+E4= 3000, "TO_MTOWBrake_TO_NoAI_3000",
+E4=4000, "TO_MTOWBrake_TO_NoAI_4000",
+E4=5000, "TO_MTOWBrake_TO_NoAI_5000",
+E4=6000, "TO_MTOWBrake_TO_NoAI_6000",
+E4=7000, "TO_MTOWBrake_TO_NoAI_7000",
+E4=8000, "TO_MTOWBrake_TO_NoAI_8000",
+E4=9000, "TO_MTOWBrake_TO_NoAI_9000",
+E4=10000, "TO_MTOWBrake_TO_NoAI_10000"), "No Table Available")</f>
+        <v>TO_MTOWBrake_TO_NoAI_6000</v>
+      </c>
       <c r="H4" s="3">
         <f>($E$4-(125*2))</f>
         <v>5750</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="32">
         <f ca="1">((I2-I6) / 2) + I6</f>
-        <v>8525</v>
+        <v>7687.5</v>
+      </c>
+      <c r="J4" s="32">
+        <f ca="1">((J2-J6) / 2) + J6</f>
+        <v>9336.6666666666679</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1323,7 +1430,7 @@
       </c>
       <c r="B5" s="39">
         <f ca="1">VLOOKUP(E8, H2:I10, 2, FALSE)</f>
-        <v>8700</v>
+        <v>7875</v>
       </c>
       <c r="D5" s="20" t="s">
         <v>107</v>
@@ -1347,22 +1454,43 @@
 E5=10000, "TO_MTOWClimb_TO_NoAI_10000"), "No Table Available")</f>
         <v>TO_MTOWClimb_TO_NoAI_5000</v>
       </c>
-      <c r="G5" s="20"/>
+      <c r="G5" s="59" t="str" cm="1">
+        <f t="array" ref="G5">IFERROR(_xlfn.IFS(E5 = 1000, "TO_MTOWBrake_TO_NoAI_1000",
+E5 = 2000, "TO_MTOWBrake_TO_NoAI_2000",
+E5= 3000, "TO_MTOWBrake_TO_NoAI_3000",
+E5=4000, "TO_MTOWBrake_TO_NoAI_4000",
+E5=5000, "TO_MTOWBrake_TO_NoAI_5000",
+E5=6000, "TO_MTOWBrake_TO_NoAI_6000",
+E5=7000, "TO_MTOWBrake_TO_NoAI_7000",
+E5=8000, "TO_MTOWBrake_TO_NoAI_8000",
+E5=9000, "TO_MTOWBrake_TO_NoAI_9000",
+E5=10000, "TO_MTOWBrake_TO_NoAI_10000"), "No Table Available")</f>
+        <v>TO_MTOWBrake_TO_NoAI_5000</v>
+      </c>
       <c r="H5" s="3">
         <f>($E$4-(125*3))</f>
         <v>5625</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="32">
         <f ca="1">((I4-I6) / 2) + I6</f>
-        <v>8612.5</v>
+        <v>7781.25</v>
+      </c>
+      <c r="J5" s="32">
+        <f ca="1">((J4-J6) / 2) + J6</f>
+        <v>9381.6666666666679</v>
+      </c>
+      <c r="L5" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="41" t="str" cm="1">
-        <f t="array" aca="1" ref="A6" ca="1">_xlfn.IFS(B5 &gt; B1, "TOW VALID FOR CONDITIONS", B5 &lt; B1, "TOW INVALID FOR CONDITIONS", B5 = B1, "TOW WARNING FOR CONDITIONS")</f>
-        <v>TOW INVALID FOR CONDITIONS</v>
-      </c>
-      <c r="B6" s="41"/>
+      <c r="A6" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" s="60">
+        <f ca="1">VLOOKUP(E8, H2:J10, 3, FALSE)</f>
+        <v>9426.6666666666679</v>
+      </c>
       <c r="D6" s="20" t="s">
         <v>108</v>
       </c>
@@ -1375,14 +1503,24 @@
         <f>($E$4-(125*4))</f>
         <v>5500</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="32">
         <f ca="1">((I10-I2) / 2) + I2</f>
-        <v>8700</v>
+        <v>7875</v>
+      </c>
+      <c r="J6" s="32">
+        <f ca="1">((J10-J2) / 2) + J2</f>
+        <v>9426.6666666666679</v>
+      </c>
+      <c r="L6" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="28"/>
+      <c r="A7" s="42" t="str" cm="1">
+        <f t="array" aca="1" ref="A7" ca="1">_xlfn.IFS(B6&gt;B5,_xlfn.IFS(B5&gt;B1,"TOW VALID FOR CONDITIONS",B5&lt;B1,"TOW INVALID FOR CONDITIONS",B5=B1,"TOW WARNING FOR CONDITIONS"),B6&lt;B5,_xlfn.IFS(B6&gt;B1,"TOW VALID FOR CONDITIONS",B6&lt;B1,"TOW INVALID FOR CONDITIONS",B6=B1,"TOW WARNING FOR CONDITIONS"))</f>
+        <v>TOW INVALID FOR CONDITIONS</v>
+      </c>
+      <c r="B7" s="42"/>
       <c r="D7" s="20" t="s">
         <v>109</v>
       </c>
@@ -1395,14 +1533,16 @@
         <f>($E$4-(125*5))</f>
         <v>5375</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="32">
         <f ca="1" xml:space="preserve"> ((I6-I8) / 2) + I8</f>
-        <v>8787.5</v>
+        <v>7968.75</v>
+      </c>
+      <c r="J7" s="32">
+        <f ca="1" xml:space="preserve"> ((J6-J8) / 2) + J8</f>
+        <v>9471.6666666666679</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="28"/>
       <c r="D8" s="20" t="s">
         <v>111</v>
       </c>
@@ -1415,9 +1555,13 @@
         <f>($E$4-(125*6))</f>
         <v>5250</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="32">
         <f ca="1">((I6-I10) / 2) + I10</f>
-        <v>8875</v>
+        <v>8062.5</v>
+      </c>
+      <c r="J8" s="32">
+        <f ca="1">((J6-J10) / 2) + J10</f>
+        <v>9516.6666666666679</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1429,9 +1573,13 @@
         <f>($E$4-(125*7))</f>
         <v>5125</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="32">
         <f ca="1">((I8-I10) / 2) + I10</f>
-        <v>8962.5</v>
+        <v>8156.25</v>
+      </c>
+      <c r="J9" s="32">
+        <f ca="1">((J8-J10) / 2) + J10</f>
+        <v>9561.6666666666679</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -1439,7 +1587,7 @@
         <v>41</v>
       </c>
       <c r="B10" s="21">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D10" s="20" t="s">
         <v>44</v>
@@ -1463,13 +1611,21 @@
         <f>($E$4-(125*8))</f>
         <v>5000</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="32">
         <f ca="1">IFERROR(
 IF(
 B10&lt;= INDEX(INDIRECT(F5), 1, 2),
 INDEX(INDIRECT(F5), 2, 2),
 VLOOKUP(B10,INDIRECT(F5),2,FALSE)), "Not within documented limits")</f>
-        <v>9050</v>
+        <v>8250</v>
+      </c>
+      <c r="J10" s="32">
+        <f ca="1">IFERROR(
+IF(
+B10&lt;= INDEX(INDIRECT(G5), 1, 2),
+INDEX(INDIRECT(G5), 2, 2),
+VLOOKUP(B10,INDIRECT(G5),2,FALSE)), "Not within documented limits")</f>
+        <v>9606.6666666666679</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -1510,7 +1666,7 @@
         <v>24.620193825305201</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H13" s="23" t="str" cm="1">
         <f t="array" ref="H13">_xlfn.IFS(
@@ -1771,8 +1927,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="H1:J1"/>
   </mergeCells>
   <conditionalFormatting sqref="D16">
     <cfRule type="expression" dxfId="6" priority="7">
@@ -1794,7 +1950,7 @@
       <formula>$B$19 = "X"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A6:B6">
+  <conditionalFormatting sqref="A7:B7">
     <cfRule type="expression" dxfId="2" priority="1">
       <formula>B1 =B5</formula>
     </cfRule>
@@ -1805,6 +1961,18 @@
       <formula>B5 &gt; B1</formula>
     </cfRule>
   </conditionalFormatting>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{E0B40120-539F-471D-AF21-7223C5F7AB09}">
+      <formula1>$L$5:$L$6</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4" xr:uid="{79E92F85-D3ED-4132-8148-5732E805C803}">
+      <formula1>$L$2:$L$3</formula1>
+    </dataValidation>
+    <dataValidation type="whole" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Aircraft MTOW Exceeded" error="The aircraft cannot, under any circumstances, takeoff with more than 10600 LBS takeoff weight." sqref="B1" xr:uid="{3FC1B319-0539-473C-BDEF-F4A8E6A43C66}">
+      <formula1>0</formula1>
+      <formula2>10601</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -1817,7 +1985,7 @@
   </sheetPr>
   <dimension ref="A1:AR443"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A223" workbookViewId="0">
       <selection sqref="A1:J1"/>
     </sheetView>
   </sheetViews>
@@ -1848,13 +2016,13 @@
       <c r="M1" s="46"/>
       <c r="N1" s="46"/>
       <c r="O1" s="9"/>
-      <c r="P1" s="41" t="s">
+      <c r="P1" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="Q1" s="41"/>
-      <c r="R1" s="41"/>
-      <c r="S1" s="41"/>
-      <c r="T1" s="41"/>
+      <c r="Q1" s="42"/>
+      <c r="R1" s="42"/>
+      <c r="S1" s="42"/>
+      <c r="T1" s="42"/>
       <c r="U1" s="9"/>
       <c r="V1" s="46" t="s">
         <v>31</v>
@@ -1871,13 +2039,13 @@
       <c r="AD1" s="46"/>
       <c r="AE1" s="46"/>
       <c r="AF1" s="46"/>
-      <c r="AH1" s="51" t="s">
+      <c r="AH1" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="AI1" s="51"/>
-      <c r="AJ1" s="51"/>
-      <c r="AK1" s="51"/>
-      <c r="AL1" s="51"/>
+      <c r="AI1" s="43"/>
+      <c r="AJ1" s="43"/>
+      <c r="AK1" s="43"/>
+      <c r="AL1" s="43"/>
       <c r="AN1" s="46" t="s">
         <v>9</v>
       </c>
@@ -1900,7 +2068,7 @@
       <c r="I2" s="50"/>
       <c r="J2" s="50"/>
       <c r="K2" s="10"/>
-      <c r="L2" s="47" t="s">
+      <c r="L2" s="51" t="s">
         <v>26</v>
       </c>
       <c r="M2" s="44"/>
@@ -1945,44 +2113,44 @@
       <c r="AR2" s="44"/>
     </row>
     <row r="3" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="47"/>
+      <c r="G3" s="47"/>
+      <c r="H3" s="47"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="47"/>
       <c r="K3" s="10"/>
       <c r="L3" s="44"/>
       <c r="M3" s="44"/>
       <c r="N3" s="44"/>
       <c r="O3" s="13"/>
-      <c r="P3" s="48" t="s">
+      <c r="P3" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="Q3" s="49"/>
-      <c r="R3" s="49"/>
-      <c r="S3" s="49"/>
-      <c r="T3" s="49"/>
+      <c r="Q3" s="52"/>
+      <c r="R3" s="52"/>
+      <c r="S3" s="52"/>
+      <c r="T3" s="52"/>
       <c r="U3" s="13"/>
-      <c r="V3" s="48" t="s">
+      <c r="V3" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="W3" s="49"/>
-      <c r="X3" s="49"/>
-      <c r="Y3" s="49"/>
-      <c r="Z3" s="49"/>
+      <c r="W3" s="52"/>
+      <c r="X3" s="52"/>
+      <c r="Y3" s="52"/>
+      <c r="Z3" s="52"/>
       <c r="AA3" s="13"/>
       <c r="AB3" s="1" t="s">
         <v>29</v>
@@ -1990,30 +2158,30 @@
       <c r="AC3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="AD3" s="48" t="s">
+      <c r="AD3" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="AE3" s="48"/>
-      <c r="AF3" s="48"/>
-      <c r="AH3" s="48" t="s">
+      <c r="AE3" s="45"/>
+      <c r="AF3" s="45"/>
+      <c r="AH3" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="AI3" s="48"/>
-      <c r="AJ3" s="48"/>
-      <c r="AK3" s="48"/>
-      <c r="AL3" s="48"/>
-      <c r="AN3" s="45" t="s">
+      <c r="AI3" s="45"/>
+      <c r="AJ3" s="45"/>
+      <c r="AK3" s="45"/>
+      <c r="AL3" s="45"/>
+      <c r="AN3" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="AO3" s="45"/>
-      <c r="AP3" s="45"/>
-      <c r="AQ3" s="45"/>
-      <c r="AR3" s="45"/>
+      <c r="AO3" s="47"/>
+      <c r="AP3" s="47"/>
+      <c r="AQ3" s="47"/>
+      <c r="AR3" s="47"/>
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A4" s="45"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="43"/>
+      <c r="A4" s="47"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="49"/>
       <c r="D4" s="2">
         <v>7800</v>
       </c>
@@ -5609,24 +5777,24 @@
       </c>
     </row>
     <row r="40" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A40" s="45" t="s">
+      <c r="A40" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B40" s="45" t="s">
+      <c r="B40" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="C40" s="42" t="s">
+      <c r="C40" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="D40" s="45" t="s">
+      <c r="D40" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="E40" s="45"/>
-      <c r="F40" s="45"/>
-      <c r="G40" s="45"/>
-      <c r="H40" s="45"/>
-      <c r="I40" s="45"/>
-      <c r="J40" s="45"/>
+      <c r="E40" s="47"/>
+      <c r="F40" s="47"/>
+      <c r="G40" s="47"/>
+      <c r="H40" s="47"/>
+      <c r="I40" s="47"/>
+      <c r="J40" s="47"/>
       <c r="K40" s="10"/>
       <c r="L40" s="10"/>
       <c r="N40" s="10"/>
@@ -5673,9 +5841,9 @@
       </c>
     </row>
     <row r="41" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A41" s="45"/>
-      <c r="B41" s="45"/>
-      <c r="C41" s="43"/>
+      <c r="A41" s="47"/>
+      <c r="B41" s="47"/>
+      <c r="C41" s="49"/>
       <c r="D41" s="2">
         <v>7800</v>
       </c>
@@ -8002,24 +8170,24 @@
       </c>
     </row>
     <row r="77" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A77" s="45" t="s">
+      <c r="A77" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B77" s="45" t="s">
+      <c r="B77" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="C77" s="42" t="s">
+      <c r="C77" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="D77" s="45" t="s">
+      <c r="D77" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="E77" s="45"/>
-      <c r="F77" s="45"/>
-      <c r="G77" s="45"/>
-      <c r="H77" s="45"/>
-      <c r="I77" s="45"/>
-      <c r="J77" s="45"/>
+      <c r="E77" s="47"/>
+      <c r="F77" s="47"/>
+      <c r="G77" s="47"/>
+      <c r="H77" s="47"/>
+      <c r="I77" s="47"/>
+      <c r="J77" s="47"/>
       <c r="K77" s="10"/>
       <c r="L77" s="10"/>
       <c r="M77" s="10"/>
@@ -8057,9 +8225,9 @@
       </c>
     </row>
     <row r="78" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A78" s="45"/>
-      <c r="B78" s="45"/>
-      <c r="C78" s="43"/>
+      <c r="A78" s="47"/>
+      <c r="B78" s="47"/>
+      <c r="C78" s="49"/>
       <c r="D78" s="2">
         <v>7800</v>
       </c>
@@ -9582,24 +9750,24 @@
       <c r="AH113" s="15"/>
     </row>
     <row r="114" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A114" s="45" t="s">
+      <c r="A114" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B114" s="45" t="s">
+      <c r="B114" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="C114" s="42" t="s">
+      <c r="C114" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="D114" s="45" t="s">
+      <c r="D114" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="E114" s="45"/>
-      <c r="F114" s="45"/>
-      <c r="G114" s="45"/>
-      <c r="H114" s="45"/>
-      <c r="I114" s="45"/>
-      <c r="J114" s="45"/>
+      <c r="E114" s="47"/>
+      <c r="F114" s="47"/>
+      <c r="G114" s="47"/>
+      <c r="H114" s="47"/>
+      <c r="I114" s="47"/>
+      <c r="J114" s="47"/>
       <c r="K114" s="10"/>
       <c r="L114" s="10"/>
       <c r="M114" s="10"/>
@@ -9624,9 +9792,9 @@
       <c r="AH114" s="15"/>
     </row>
     <row r="115" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A115" s="45"/>
-      <c r="B115" s="45"/>
-      <c r="C115" s="43"/>
+      <c r="A115" s="47"/>
+      <c r="B115" s="47"/>
+      <c r="C115" s="49"/>
       <c r="D115" s="2">
         <v>7800</v>
       </c>
@@ -11003,24 +11171,24 @@
       <c r="AH150" s="15"/>
     </row>
     <row r="151" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A151" s="45" t="s">
+      <c r="A151" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B151" s="45" t="s">
+      <c r="B151" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="C151" s="42" t="s">
+      <c r="C151" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="D151" s="45" t="s">
+      <c r="D151" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="E151" s="45"/>
-      <c r="F151" s="45"/>
-      <c r="G151" s="45"/>
-      <c r="H151" s="45"/>
-      <c r="I151" s="45"/>
-      <c r="J151" s="45"/>
+      <c r="E151" s="47"/>
+      <c r="F151" s="47"/>
+      <c r="G151" s="47"/>
+      <c r="H151" s="47"/>
+      <c r="I151" s="47"/>
+      <c r="J151" s="47"/>
       <c r="K151" s="10"/>
       <c r="L151" s="10"/>
       <c r="M151" s="10"/>
@@ -11045,9 +11213,9 @@
       <c r="AH151" s="15"/>
     </row>
     <row r="152" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A152" s="45"/>
-      <c r="B152" s="45"/>
-      <c r="C152" s="43"/>
+      <c r="A152" s="47"/>
+      <c r="B152" s="47"/>
+      <c r="C152" s="49"/>
       <c r="D152" s="2">
         <v>7800</v>
       </c>
@@ -12422,24 +12590,24 @@
       <c r="AF187" s="13"/>
     </row>
     <row r="188" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A188" s="45" t="s">
+      <c r="A188" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B188" s="45" t="s">
+      <c r="B188" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="C188" s="42" t="s">
+      <c r="C188" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="D188" s="45" t="s">
+      <c r="D188" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="E188" s="45"/>
-      <c r="F188" s="45"/>
-      <c r="G188" s="45"/>
-      <c r="H188" s="45"/>
-      <c r="I188" s="45"/>
-      <c r="J188" s="45"/>
+      <c r="E188" s="47"/>
+      <c r="F188" s="47"/>
+      <c r="G188" s="47"/>
+      <c r="H188" s="47"/>
+      <c r="I188" s="47"/>
+      <c r="J188" s="47"/>
       <c r="K188" s="10"/>
       <c r="L188" s="10"/>
       <c r="M188" s="10"/>
@@ -12463,9 +12631,9 @@
       <c r="AF188" s="10"/>
     </row>
     <row r="189" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A189" s="45"/>
-      <c r="B189" s="45"/>
-      <c r="C189" s="43"/>
+      <c r="A189" s="47"/>
+      <c r="B189" s="47"/>
+      <c r="C189" s="49"/>
       <c r="D189" s="2">
         <v>7800</v>
       </c>
@@ -13888,24 +14056,24 @@
       <c r="AF224" s="13"/>
     </row>
     <row r="225" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A225" s="45" t="s">
+      <c r="A225" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B225" s="45" t="s">
+      <c r="B225" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="C225" s="42" t="s">
+      <c r="C225" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="D225" s="45" t="s">
+      <c r="D225" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="E225" s="45"/>
-      <c r="F225" s="45"/>
-      <c r="G225" s="45"/>
-      <c r="H225" s="45"/>
-      <c r="I225" s="45"/>
-      <c r="J225" s="45"/>
+      <c r="E225" s="47"/>
+      <c r="F225" s="47"/>
+      <c r="G225" s="47"/>
+      <c r="H225" s="47"/>
+      <c r="I225" s="47"/>
+      <c r="J225" s="47"/>
       <c r="K225" s="10"/>
       <c r="L225" s="10"/>
       <c r="M225" s="10"/>
@@ -13929,9 +14097,9 @@
       <c r="AF225" s="10"/>
     </row>
     <row r="226" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A226" s="45"/>
-      <c r="B226" s="45"/>
-      <c r="C226" s="43"/>
+      <c r="A226" s="47"/>
+      <c r="B226" s="47"/>
+      <c r="C226" s="49"/>
       <c r="D226" s="2">
         <v>7800</v>
       </c>
@@ -15354,24 +15522,24 @@
       <c r="AF261" s="13"/>
     </row>
     <row r="262" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A262" s="45" t="s">
+      <c r="A262" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B262" s="45" t="s">
+      <c r="B262" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="C262" s="42" t="s">
+      <c r="C262" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="D262" s="45" t="s">
+      <c r="D262" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="E262" s="45"/>
-      <c r="F262" s="45"/>
-      <c r="G262" s="45"/>
-      <c r="H262" s="45"/>
-      <c r="I262" s="45"/>
-      <c r="J262" s="45"/>
+      <c r="E262" s="47"/>
+      <c r="F262" s="47"/>
+      <c r="G262" s="47"/>
+      <c r="H262" s="47"/>
+      <c r="I262" s="47"/>
+      <c r="J262" s="47"/>
       <c r="K262" s="10"/>
       <c r="L262" s="10"/>
       <c r="M262" s="10"/>
@@ -15395,9 +15563,9 @@
       <c r="AF262" s="10"/>
     </row>
     <row r="263" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A263" s="45"/>
-      <c r="B263" s="45"/>
-      <c r="C263" s="43"/>
+      <c r="A263" s="47"/>
+      <c r="B263" s="47"/>
+      <c r="C263" s="49"/>
       <c r="D263" s="2">
         <v>7800</v>
       </c>
@@ -16820,24 +16988,24 @@
       <c r="AF298" s="13"/>
     </row>
     <row r="299" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A299" s="45" t="s">
+      <c r="A299" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B299" s="45" t="s">
+      <c r="B299" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="C299" s="42" t="s">
+      <c r="C299" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="D299" s="45" t="s">
+      <c r="D299" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="E299" s="45"/>
-      <c r="F299" s="45"/>
-      <c r="G299" s="45"/>
-      <c r="H299" s="45"/>
-      <c r="I299" s="45"/>
-      <c r="J299" s="45"/>
+      <c r="E299" s="47"/>
+      <c r="F299" s="47"/>
+      <c r="G299" s="47"/>
+      <c r="H299" s="47"/>
+      <c r="I299" s="47"/>
+      <c r="J299" s="47"/>
       <c r="K299" s="10"/>
       <c r="L299" s="10"/>
       <c r="M299" s="10"/>
@@ -16861,9 +17029,9 @@
       <c r="AF299" s="10"/>
     </row>
     <row r="300" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A300" s="45"/>
-      <c r="B300" s="45"/>
-      <c r="C300" s="43"/>
+      <c r="A300" s="47"/>
+      <c r="B300" s="47"/>
+      <c r="C300" s="49"/>
       <c r="D300" s="2">
         <v>7800</v>
       </c>
@@ -18286,24 +18454,24 @@
       <c r="AF335" s="13"/>
     </row>
     <row r="336" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A336" s="45" t="s">
+      <c r="A336" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B336" s="45" t="s">
+      <c r="B336" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="C336" s="42" t="s">
+      <c r="C336" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="D336" s="45" t="s">
+      <c r="D336" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="E336" s="45"/>
-      <c r="F336" s="45"/>
-      <c r="G336" s="45"/>
-      <c r="H336" s="45"/>
-      <c r="I336" s="45"/>
-      <c r="J336" s="45"/>
+      <c r="E336" s="47"/>
+      <c r="F336" s="47"/>
+      <c r="G336" s="47"/>
+      <c r="H336" s="47"/>
+      <c r="I336" s="47"/>
+      <c r="J336" s="47"/>
       <c r="K336" s="10"/>
       <c r="L336" s="10"/>
       <c r="M336" s="10"/>
@@ -18327,9 +18495,9 @@
       <c r="AF336" s="10"/>
     </row>
     <row r="337" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A337" s="45"/>
-      <c r="B337" s="45"/>
-      <c r="C337" s="43"/>
+      <c r="A337" s="47"/>
+      <c r="B337" s="47"/>
+      <c r="C337" s="49"/>
       <c r="D337" s="2">
         <v>7800</v>
       </c>
@@ -19752,24 +19920,24 @@
       <c r="AF372" s="13"/>
     </row>
     <row r="373" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A373" s="45" t="s">
+      <c r="A373" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B373" s="45" t="s">
+      <c r="B373" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="C373" s="42" t="s">
+      <c r="C373" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="D373" s="45" t="s">
+      <c r="D373" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="E373" s="45"/>
-      <c r="F373" s="45"/>
-      <c r="G373" s="45"/>
-      <c r="H373" s="45"/>
-      <c r="I373" s="45"/>
-      <c r="J373" s="45"/>
+      <c r="E373" s="47"/>
+      <c r="F373" s="47"/>
+      <c r="G373" s="47"/>
+      <c r="H373" s="47"/>
+      <c r="I373" s="47"/>
+      <c r="J373" s="47"/>
       <c r="K373" s="10"/>
       <c r="L373" s="10"/>
       <c r="M373" s="10"/>
@@ -19793,9 +19961,9 @@
       <c r="AF373" s="10"/>
     </row>
     <row r="374" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A374" s="45"/>
-      <c r="B374" s="45"/>
-      <c r="C374" s="43"/>
+      <c r="A374" s="47"/>
+      <c r="B374" s="47"/>
+      <c r="C374" s="49"/>
       <c r="D374" s="2">
         <v>7800</v>
       </c>
@@ -21302,24 +21470,24 @@
       <c r="AF409" s="13"/>
     </row>
     <row r="410" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A410" s="45" t="s">
+      <c r="A410" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="B410" s="45" t="s">
+      <c r="B410" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="C410" s="42" t="s">
+      <c r="C410" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="D410" s="45" t="s">
+      <c r="D410" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="E410" s="45"/>
-      <c r="F410" s="45"/>
-      <c r="G410" s="45"/>
-      <c r="H410" s="45"/>
-      <c r="I410" s="45"/>
-      <c r="J410" s="45"/>
+      <c r="E410" s="47"/>
+      <c r="F410" s="47"/>
+      <c r="G410" s="47"/>
+      <c r="H410" s="47"/>
+      <c r="I410" s="47"/>
+      <c r="J410" s="47"/>
       <c r="K410" s="10"/>
       <c r="L410" s="10"/>
       <c r="M410" s="10"/>
@@ -21343,9 +21511,9 @@
       <c r="AF410" s="10"/>
     </row>
     <row r="411" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A411" s="45"/>
-      <c r="B411" s="45"/>
-      <c r="C411" s="43"/>
+      <c r="A411" s="47"/>
+      <c r="B411" s="47"/>
+      <c r="C411" s="49"/>
       <c r="D411" s="2">
         <v>7800</v>
       </c>
@@ -22699,6 +22867,79 @@
     </row>
   </sheetData>
   <mergeCells count="89">
+    <mergeCell ref="C336:C337"/>
+    <mergeCell ref="C299:C300"/>
+    <mergeCell ref="C262:C263"/>
+    <mergeCell ref="C225:C226"/>
+    <mergeCell ref="C188:C189"/>
+    <mergeCell ref="A261:J261"/>
+    <mergeCell ref="A262:A263"/>
+    <mergeCell ref="B262:B263"/>
+    <mergeCell ref="D262:J262"/>
+    <mergeCell ref="A223:J223"/>
+    <mergeCell ref="A224:J224"/>
+    <mergeCell ref="A225:A226"/>
+    <mergeCell ref="B225:B226"/>
+    <mergeCell ref="D225:J225"/>
+    <mergeCell ref="A112:J112"/>
+    <mergeCell ref="A113:J113"/>
+    <mergeCell ref="A114:A115"/>
+    <mergeCell ref="B114:B115"/>
+    <mergeCell ref="D114:J114"/>
+    <mergeCell ref="C114:C115"/>
+    <mergeCell ref="A75:J75"/>
+    <mergeCell ref="A76:J76"/>
+    <mergeCell ref="A77:A78"/>
+    <mergeCell ref="B77:B78"/>
+    <mergeCell ref="D77:J77"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="AN1:AR1"/>
+    <mergeCell ref="AN2:AR2"/>
+    <mergeCell ref="AN3:AR3"/>
+    <mergeCell ref="A38:J38"/>
+    <mergeCell ref="A39:J39"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="L2:N3"/>
+    <mergeCell ref="P1:T1"/>
+    <mergeCell ref="P2:T2"/>
+    <mergeCell ref="P3:T3"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="V2:Z2"/>
+    <mergeCell ref="V3:Z3"/>
+    <mergeCell ref="AB1:AF1"/>
+    <mergeCell ref="AB2:AF2"/>
+    <mergeCell ref="AD3:AF3"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="D40:J40"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="D3:J3"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="A149:J149"/>
+    <mergeCell ref="A150:J150"/>
+    <mergeCell ref="A151:A152"/>
+    <mergeCell ref="B151:B152"/>
+    <mergeCell ref="D151:J151"/>
+    <mergeCell ref="C151:C152"/>
+    <mergeCell ref="A186:J186"/>
+    <mergeCell ref="A187:J187"/>
+    <mergeCell ref="A188:A189"/>
+    <mergeCell ref="B188:B189"/>
+    <mergeCell ref="D188:J188"/>
+    <mergeCell ref="A410:A411"/>
+    <mergeCell ref="B410:B411"/>
+    <mergeCell ref="D410:J410"/>
+    <mergeCell ref="A371:J371"/>
+    <mergeCell ref="A372:J372"/>
+    <mergeCell ref="A373:A374"/>
+    <mergeCell ref="B373:B374"/>
+    <mergeCell ref="D373:J373"/>
+    <mergeCell ref="C410:C411"/>
+    <mergeCell ref="C373:C374"/>
     <mergeCell ref="AH1:AL1"/>
     <mergeCell ref="AH2:AL2"/>
     <mergeCell ref="AH3:AL3"/>
@@ -22715,79 +22956,6 @@
     <mergeCell ref="A297:J297"/>
     <mergeCell ref="A298:J298"/>
     <mergeCell ref="A260:J260"/>
-    <mergeCell ref="A410:A411"/>
-    <mergeCell ref="B410:B411"/>
-    <mergeCell ref="D410:J410"/>
-    <mergeCell ref="A371:J371"/>
-    <mergeCell ref="A372:J372"/>
-    <mergeCell ref="A373:A374"/>
-    <mergeCell ref="B373:B374"/>
-    <mergeCell ref="D373:J373"/>
-    <mergeCell ref="C410:C411"/>
-    <mergeCell ref="C373:C374"/>
-    <mergeCell ref="A186:J186"/>
-    <mergeCell ref="A187:J187"/>
-    <mergeCell ref="A188:A189"/>
-    <mergeCell ref="B188:B189"/>
-    <mergeCell ref="D188:J188"/>
-    <mergeCell ref="A149:J149"/>
-    <mergeCell ref="A150:J150"/>
-    <mergeCell ref="A151:A152"/>
-    <mergeCell ref="B151:B152"/>
-    <mergeCell ref="D151:J151"/>
-    <mergeCell ref="C151:C152"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="D40:J40"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="D3:J3"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="AN1:AR1"/>
-    <mergeCell ref="AN2:AR2"/>
-    <mergeCell ref="AN3:AR3"/>
-    <mergeCell ref="A38:J38"/>
-    <mergeCell ref="A39:J39"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="L2:N3"/>
-    <mergeCell ref="P1:T1"/>
-    <mergeCell ref="P2:T2"/>
-    <mergeCell ref="P3:T3"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="V2:Z2"/>
-    <mergeCell ref="V3:Z3"/>
-    <mergeCell ref="AB1:AF1"/>
-    <mergeCell ref="AB2:AF2"/>
-    <mergeCell ref="AD3:AF3"/>
-    <mergeCell ref="A75:J75"/>
-    <mergeCell ref="A76:J76"/>
-    <mergeCell ref="A77:A78"/>
-    <mergeCell ref="B77:B78"/>
-    <mergeCell ref="D77:J77"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="A112:J112"/>
-    <mergeCell ref="A113:J113"/>
-    <mergeCell ref="A114:A115"/>
-    <mergeCell ref="B114:B115"/>
-    <mergeCell ref="D114:J114"/>
-    <mergeCell ref="C114:C115"/>
-    <mergeCell ref="C336:C337"/>
-    <mergeCell ref="C299:C300"/>
-    <mergeCell ref="C262:C263"/>
-    <mergeCell ref="C225:C226"/>
-    <mergeCell ref="C188:C189"/>
-    <mergeCell ref="A261:J261"/>
-    <mergeCell ref="A262:A263"/>
-    <mergeCell ref="B262:B263"/>
-    <mergeCell ref="D262:J262"/>
-    <mergeCell ref="A223:J223"/>
-    <mergeCell ref="A224:J224"/>
-    <mergeCell ref="A225:A226"/>
-    <mergeCell ref="B225:B226"/>
-    <mergeCell ref="D225:J225"/>
   </mergeCells>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -22802,7 +22970,7 @@
   </sheetPr>
   <dimension ref="A1:G272"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A106" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -22816,22 +22984,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
-        <v>117</v>
-      </c>
-      <c r="B1" s="53"/>
+      <c r="A1" s="53" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="54"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="55" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="55"/>
+      <c r="B2" s="56"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="56" t="s">
-        <v>115</v>
-      </c>
-      <c r="B3" s="57">
+      <c r="A3" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" s="41">
         <v>49</v>
       </c>
     </row>
@@ -22908,22 +23076,22 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="52" t="s">
-        <v>117</v>
-      </c>
-      <c r="B14" s="53"/>
+      <c r="A14" s="53" t="s">
+        <v>116</v>
+      </c>
+      <c r="B14" s="54"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="54" t="s">
+      <c r="A15" s="55" t="s">
         <v>64</v>
       </c>
-      <c r="B15" s="55"/>
+      <c r="B15" s="56"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="56" t="s">
-        <v>115</v>
-      </c>
-      <c r="B16" s="57">
+      <c r="A16" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="B16" s="41">
         <v>47</v>
       </c>
     </row>
@@ -23004,10 +23172,10 @@
       <c r="B26"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="52" t="s">
-        <v>117</v>
-      </c>
-      <c r="B27" s="53"/>
+      <c r="A27" s="53" t="s">
+        <v>116</v>
+      </c>
+      <c r="B27" s="54"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="44" t="s">
@@ -23016,10 +23184,10 @@
       <c r="B28" s="44"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="56" t="s">
-        <v>115</v>
-      </c>
-      <c r="B29" s="57">
+      <c r="A29" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="B29" s="41">
         <v>44</v>
       </c>
     </row>
@@ -23108,10 +23276,10 @@
       <c r="B40"/>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="52" t="s">
-        <v>117</v>
-      </c>
-      <c r="B41" s="53"/>
+      <c r="A41" s="53" t="s">
+        <v>116</v>
+      </c>
+      <c r="B41" s="54"/>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="44" t="s">
@@ -23120,10 +23288,10 @@
       <c r="B42" s="44"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="56" t="s">
-        <v>115</v>
-      </c>
-      <c r="B43" s="57">
+      <c r="A43" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="B43" s="41">
         <v>41</v>
       </c>
     </row>
@@ -23220,10 +23388,10 @@
       <c r="B55"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="52" t="s">
-        <v>117</v>
-      </c>
-      <c r="B56" s="53"/>
+      <c r="A56" s="53" t="s">
+        <v>116</v>
+      </c>
+      <c r="B56" s="54"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="44" t="s">
@@ -23232,10 +23400,10 @@
       <c r="B57" s="44"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="56" t="s">
-        <v>115</v>
-      </c>
-      <c r="B58" s="57">
+      <c r="A58" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="B58" s="41">
         <v>39</v>
       </c>
     </row>
@@ -23332,10 +23500,10 @@
       <c r="B70"/>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="52" t="s">
-        <v>117</v>
-      </c>
-      <c r="B71" s="53"/>
+      <c r="A71" s="53" t="s">
+        <v>116</v>
+      </c>
+      <c r="B71" s="54"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="44" t="s">
@@ -23344,10 +23512,10 @@
       <c r="B72" s="44"/>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="56" t="s">
-        <v>115</v>
-      </c>
-      <c r="B73" s="57">
+      <c r="A73" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="B73" s="41">
         <v>33</v>
       </c>
     </row>
@@ -23468,10 +23636,10 @@
       <c r="B88"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="52" t="s">
-        <v>117</v>
-      </c>
-      <c r="B89" s="53"/>
+      <c r="A89" s="53" t="s">
+        <v>116</v>
+      </c>
+      <c r="B89" s="54"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="44" t="s">
@@ -23480,10 +23648,10 @@
       <c r="B90" s="44"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="56" t="s">
-        <v>115</v>
-      </c>
-      <c r="B91" s="57">
+      <c r="A91" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="B91" s="41">
         <v>30</v>
       </c>
     </row>
@@ -23620,10 +23788,10 @@
       <c r="B108"/>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="52" t="s">
-        <v>117</v>
-      </c>
-      <c r="B109" s="53"/>
+      <c r="A109" s="53" t="s">
+        <v>116</v>
+      </c>
+      <c r="B109" s="54"/>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="44" t="s">
@@ -23632,10 +23800,10 @@
       <c r="B110" s="44"/>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="56" t="s">
-        <v>115</v>
-      </c>
-      <c r="B111" s="57">
+      <c r="A111" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="B111" s="41">
         <v>26</v>
       </c>
     </row>
@@ -23788,10 +23956,10 @@
       <c r="B130"/>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="52" t="s">
-        <v>117</v>
-      </c>
-      <c r="B131" s="53"/>
+      <c r="A131" s="53" t="s">
+        <v>116</v>
+      </c>
+      <c r="B131" s="54"/>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="44" t="s">
@@ -23800,10 +23968,10 @@
       <c r="B132" s="44"/>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="56" t="s">
-        <v>115</v>
-      </c>
-      <c r="B133" s="57">
+      <c r="A133" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="B133" s="41">
         <v>22</v>
       </c>
     </row>
@@ -23956,10 +24124,10 @@
       <c r="B152"/>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" s="52" t="s">
-        <v>117</v>
-      </c>
-      <c r="B153" s="53"/>
+      <c r="A153" s="53" t="s">
+        <v>116</v>
+      </c>
+      <c r="B153" s="54"/>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="44" t="s">
@@ -23968,10 +24136,10 @@
       <c r="B154" s="44"/>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" s="56" t="s">
-        <v>115</v>
-      </c>
-      <c r="B155" s="57">
+      <c r="A155" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="B155" s="41">
         <v>19</v>
       </c>
     </row>
@@ -24117,10 +24285,10 @@
       <c r="G173" s="31"/>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A174" s="52" t="s">
-        <v>117</v>
-      </c>
-      <c r="B174" s="53"/>
+      <c r="A174" s="53" t="s">
+        <v>116</v>
+      </c>
+      <c r="B174" s="54"/>
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" s="44" t="s">
@@ -24129,10 +24297,10 @@
       <c r="B175" s="44"/>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A176" s="56" t="s">
-        <v>115</v>
-      </c>
-      <c r="B176" s="57">
+      <c r="A176" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="B176" s="41">
         <v>15</v>
       </c>
     </row>
@@ -24285,10 +24453,10 @@
       <c r="B195"/>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A196" s="52" t="s">
-        <v>117</v>
-      </c>
-      <c r="B196" s="53"/>
+      <c r="A196" s="53" t="s">
+        <v>116</v>
+      </c>
+      <c r="B196" s="54"/>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="44" t="s">
@@ -24297,10 +24465,10 @@
       <c r="B197" s="44"/>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A198" s="56" t="s">
-        <v>115</v>
-      </c>
-      <c r="B198" s="57">
+      <c r="A198" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="B198" s="41">
         <v>10</v>
       </c>
     </row>
@@ -24468,6 +24636,16 @@
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
     <mergeCell ref="A71:B71"/>
     <mergeCell ref="A175:B175"/>
     <mergeCell ref="A196:B196"/>
@@ -24482,16 +24660,6 @@
     <mergeCell ref="A132:B132"/>
     <mergeCell ref="A153:B153"/>
     <mergeCell ref="A154:B154"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A27:B27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -24505,8 +24673,8 @@
   </sheetPr>
   <dimension ref="A1:B313"/>
   <sheetViews>
-    <sheetView topLeftCell="A184" workbookViewId="0">
-      <selection activeCell="A251" sqref="A251:B251"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G244" sqref="F243:G244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24516,10 +24684,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
-        <v>116</v>
-      </c>
-      <c r="B1" s="53"/>
+      <c r="A1" s="53" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="54"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="44" t="s">
@@ -24528,10 +24696,10 @@
       <c r="B2" s="44"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="56" t="s">
-        <v>115</v>
-      </c>
-      <c r="B3" s="57">
+      <c r="A3" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" s="41">
         <v>50</v>
       </c>
     </row>
@@ -24571,10 +24739,10 @@
       <c r="B8" s="33"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="52" t="s">
-        <v>116</v>
-      </c>
-      <c r="B9" s="53"/>
+      <c r="A9" s="53" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9" s="54"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="44" t="s">
@@ -24583,10 +24751,10 @@
       <c r="B10" s="44"/>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="56" t="s">
-        <v>115</v>
-      </c>
-      <c r="B11" s="57">
+      <c r="A11" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" s="41">
         <v>44</v>
       </c>
     </row>
@@ -24666,10 +24834,10 @@
       <c r="B20" s="33"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="52" t="s">
-        <v>116</v>
-      </c>
-      <c r="B21" s="53"/>
+      <c r="A21" s="53" t="s">
+        <v>115</v>
+      </c>
+      <c r="B21" s="54"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="44" t="s">
@@ -24678,10 +24846,10 @@
       <c r="B22" s="44"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="56" t="s">
-        <v>115</v>
-      </c>
-      <c r="B23" s="57">
+      <c r="A23" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="B23" s="41">
         <v>38</v>
       </c>
     </row>
@@ -24796,10 +24964,10 @@
       <c r="B36" s="33"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="52" t="s">
-        <v>116</v>
-      </c>
-      <c r="B37" s="53"/>
+      <c r="A37" s="53" t="s">
+        <v>115</v>
+      </c>
+      <c r="B37" s="54"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="44" t="s">
@@ -24808,10 +24976,10 @@
       <c r="B38" s="44"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="56" t="s">
-        <v>115</v>
-      </c>
-      <c r="B39" s="57">
+      <c r="A39" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="B39" s="41">
         <v>31</v>
       </c>
     </row>
@@ -24972,10 +25140,10 @@
       <c r="B57" s="33"/>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="52" t="s">
-        <v>116</v>
-      </c>
-      <c r="B58" s="53"/>
+      <c r="A58" s="53" t="s">
+        <v>115</v>
+      </c>
+      <c r="B58" s="54"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="44" t="s">
@@ -24984,10 +25152,10 @@
       <c r="B59" s="44"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="56" t="s">
-        <v>115</v>
-      </c>
-      <c r="B60" s="57">
+      <c r="A60" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="B60" s="41">
         <v>24</v>
       </c>
     </row>
@@ -25192,10 +25360,10 @@
       <c r="B83" s="33"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="52" t="s">
-        <v>116</v>
-      </c>
-      <c r="B84" s="53"/>
+      <c r="A84" s="53" t="s">
+        <v>115</v>
+      </c>
+      <c r="B84" s="54"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="44" t="s">
@@ -25204,10 +25372,10 @@
       <c r="B85" s="44"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="56" t="s">
-        <v>115</v>
-      </c>
-      <c r="B86" s="57">
+      <c r="A86" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="B86" s="41">
         <v>18</v>
       </c>
     </row>
@@ -25448,10 +25616,10 @@
       <c r="B113" s="33"/>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="52" t="s">
-        <v>116</v>
-      </c>
-      <c r="B114" s="53"/>
+      <c r="A114" s="53" t="s">
+        <v>115</v>
+      </c>
+      <c r="B114" s="54"/>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="44" t="s">
@@ -25460,10 +25628,10 @@
       <c r="B115" s="44"/>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="56" t="s">
-        <v>115</v>
-      </c>
-      <c r="B116" s="57">
+      <c r="A116" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="B116" s="41">
         <v>11</v>
       </c>
     </row>
@@ -25749,10 +25917,10 @@
       <c r="B148" s="33"/>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" s="52" t="s">
-        <v>116</v>
-      </c>
-      <c r="B149" s="53"/>
+      <c r="A149" s="53" t="s">
+        <v>115</v>
+      </c>
+      <c r="B149" s="54"/>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="44" t="s">
@@ -25761,10 +25929,10 @@
       <c r="B150" s="44"/>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" s="56" t="s">
-        <v>115</v>
-      </c>
-      <c r="B151" s="57">
+      <c r="A151" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="B151" s="41">
         <v>-2</v>
       </c>
     </row>
@@ -26149,10 +26317,10 @@
       <c r="B194" s="33"/>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A195" s="52" t="s">
-        <v>116</v>
-      </c>
-      <c r="B195" s="53"/>
+      <c r="A195" s="53" t="s">
+        <v>115</v>
+      </c>
+      <c r="B195" s="54"/>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" s="44" t="s">
@@ -26161,10 +26329,10 @@
       <c r="B196" s="44"/>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A197" s="56" t="s">
-        <v>115</v>
-      </c>
-      <c r="B197" s="57">
+      <c r="A197" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="B197" s="41">
         <v>-14</v>
       </c>
     </row>
@@ -26639,10 +26807,10 @@
       <c r="B250" s="33"/>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A251" s="52" t="s">
-        <v>116</v>
-      </c>
-      <c r="B251" s="53"/>
+      <c r="A251" s="53" t="s">
+        <v>115</v>
+      </c>
+      <c r="B251" s="54"/>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" s="44" t="s">
@@ -26651,10 +26819,10 @@
       <c r="B252" s="44"/>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A253" s="56" t="s">
-        <v>115</v>
-      </c>
-      <c r="B253" s="57">
+      <c r="A253" s="40" t="s">
+        <v>114</v>
+      </c>
+      <c r="B253" s="41">
         <v>-26</v>
       </c>
     </row>
@@ -27199,26 +27367,26 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A150:B150"/>
+    <mergeCell ref="A195:B195"/>
+    <mergeCell ref="A196:B196"/>
+    <mergeCell ref="A251:B251"/>
+    <mergeCell ref="A252:B252"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A114:B114"/>
+    <mergeCell ref="A115:B115"/>
+    <mergeCell ref="A149:B149"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A114:B114"/>
-    <mergeCell ref="A115:B115"/>
-    <mergeCell ref="A149:B149"/>
-    <mergeCell ref="A150:B150"/>
-    <mergeCell ref="A195:B195"/>
-    <mergeCell ref="A196:B196"/>
-    <mergeCell ref="A251:B251"/>
-    <mergeCell ref="A252:B252"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>